<commit_message>
Capacity Problem fixed + DA Model running
</commit_message>
<xml_diff>
--- a/Data/ReferenceCase/OPEX.xlsx
+++ b/Data/ReferenceCase/OPEX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee65a08843967445/Desktop/Master Ordner Konsti/03_Studium/Master/Sustainable Energy - Energy Systems Analysis/Masterarbeit/MasterThesis/Data/Reference Case/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee65a08843967445/Desktop/Master Ordner Konsti/03_Studium/Master/Sustainable Energy - Energy Systems Analysis/Masterarbeit/MasterThesis/Data/ReferenceCase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{62F7584F-92F1-43AB-8684-75104CC73B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCED0693-8030-41EC-9474-69C4A3D61351}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{62F7584F-92F1-43AB-8684-75104CC73B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E352D2A0-54E8-4635-ACF7-451736D1FB39}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A6326503-DCBD-45B8-99ED-538B88B01DFC}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,8 +800,7 @@
         <v>18</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added first version of battery optimization and regression
</commit_message>
<xml_diff>
--- a/Data/ReferenceCase/OPEX.xlsx
+++ b/Data/ReferenceCase/OPEX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee65a08843967445/Desktop/Master Ordner Konsti/03_Studium/Master/Sustainable Energy - Energy Systems Analysis/Masterarbeit/MasterThesis/Data/ReferenceCase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{62F7584F-92F1-43AB-8684-75104CC73B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E352D2A0-54E8-4635-ACF7-451736D1FB39}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{62F7584F-92F1-43AB-8684-75104CC73B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0453B25-F5F7-4F31-9017-BB102B2132EE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A6326503-DCBD-45B8-99ED-538B88B01DFC}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{A6326503-DCBD-45B8-99ED-538B88B01DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,32 +71,6 @@
     <t>Fuel Cost [€/MWh]</t>
   </si>
   <si>
-    <r>
-      <t>CO2 emissions [t/MWh</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
     <t>CO2 Price [€/t]</t>
   </si>
   <si>
@@ -119,13 +93,20 @@
   </si>
   <si>
     <t>Total OPEX [€/GWh]</t>
+  </si>
+  <si>
+    <t>CO2 emissions [t/MWh]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,14 +115,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -166,16 +139,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -512,7 +488,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -524,14 +500,15 @@
     <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -543,13 +520,13 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -570,9 +547,9 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <v>125</v>
-      </c>
-      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="H2" s="3">
         <f>(E2+F2*G2)*1000</f>
         <v>0</v>
       </c>
@@ -588,16 +565,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E10" si="0">C3/D3</f>
+        <f t="shared" ref="E3:E13" si="0">C3/D3</f>
         <v>0</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>125</v>
-      </c>
-      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="H3" s="3">
         <f t="shared" ref="H3:H13" si="1">(E3+F3*G3)*1000</f>
         <v>0</v>
       </c>
@@ -620,9 +597,9 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>125</v>
-      </c>
-      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="H4" s="3">
         <f t="shared" si="1"/>
         <v>77981.65137614678</v>
       </c>
@@ -642,14 +619,14 @@
         <v>5.8974358974358969</v>
       </c>
       <c r="F5" s="2">
-        <v>0.3987</v>
+        <v>1.0489999999999999</v>
       </c>
       <c r="G5" s="1">
-        <v>125</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>55734.935897435898</v>
+        <v>100</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="1"/>
+        <v>110797.43589743589</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -667,19 +644,19 @@
         <v>28.999999999999996</v>
       </c>
       <c r="F6" s="2">
-        <v>0.3382</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="G6" s="1">
-        <v>125</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>71274.999999999985</v>
+        <v>100</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>115700</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>27</v>
@@ -692,19 +669,19 @@
         <v>67.5</v>
       </c>
       <c r="F7" s="2">
-        <v>0.20080000000000001</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="G7" s="1">
-        <v>125</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>92600</v>
+        <v>100</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="1"/>
+        <v>103300</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>150</v>
@@ -720,9 +697,9 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>125</v>
-      </c>
-      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>375000</v>
       </c>
@@ -745,9 +722,9 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>125</v>
-      </c>
-      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="H9" s="3">
         <f t="shared" si="1"/>
         <v>22857.142857142859</v>
       </c>
@@ -770,37 +747,87 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>125</v>
-      </c>
-      <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>100</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>100</v>
+      </c>
+      <c r="H12" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13">
-        <v>100000</v>
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>0.4</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="F13" s="2">
+        <f>F7*(266/201)</f>
+        <v>0.47377114427860695</v>
+      </c>
+      <c r="G13" s="1">
+        <v>100</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="1"/>
+        <v>297377.11442786071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>